<commit_message>
reivsed  model of  syb data and save individual series into json
Reduced the file size by storing only the footnote and source id in each record,
adding their descriptions to the root level of the tree
</commit_message>
<xml_diff>
--- a/data/unsd/UNSYB/input/SYB series mapping to DSD.xlsx
+++ b/data/unsd/UNSYB/input/SYB series mapping to DSD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\data\unsd\UNSYB\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C052A6F2-C48B-4BAF-BF67-C4E221B26301}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E8795-C995-47A6-B208-FE75B8712ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SYB series mapping to DSD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="676">
   <si>
     <t>seriesCode</t>
   </si>
@@ -2906,30 +2906,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H106" sqref="H106"/>
+      <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="112.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="112.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="27" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="15.6640625" customWidth="1"/>
+    <col min="19" max="27" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>558</v>
       </c>
@@ -3012,7 +3011,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>405</v>
       </c>
@@ -3047,7 +3046,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>381</v>
       </c>
@@ -3082,7 +3081,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>407</v>
       </c>
@@ -3117,7 +3116,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>383</v>
       </c>
@@ -3152,7 +3151,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>409</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>385</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -3247,12 +3246,6 @@
       <c r="J8">
         <v>3</v>
       </c>
-      <c r="X8" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>592</v>
-      </c>
       <c r="Z8" t="s">
         <v>634</v>
       </c>
@@ -3260,7 +3253,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>82</v>
       </c>
@@ -3285,12 +3278,6 @@
       <c r="J9">
         <v>3</v>
       </c>
-      <c r="X9" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>592</v>
-      </c>
       <c r="Z9" t="s">
         <v>637</v>
       </c>
@@ -3298,7 +3285,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>84</v>
       </c>
@@ -3323,12 +3310,6 @@
       <c r="J10">
         <v>3</v>
       </c>
-      <c r="X10" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>592</v>
-      </c>
       <c r="Z10" t="s">
         <v>638</v>
       </c>
@@ -3336,7 +3317,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>194</v>
       </c>
@@ -3364,14 +3345,8 @@
       <c r="Q11" t="s">
         <v>437</v>
       </c>
-      <c r="X11" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>196</v>
       </c>
@@ -3399,14 +3374,8 @@
       <c r="Q12" t="s">
         <v>438</v>
       </c>
-      <c r="X12" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>198</v>
       </c>
@@ -3434,14 +3403,8 @@
       <c r="Q13" t="s">
         <v>418</v>
       </c>
-      <c r="X13" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y13" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -3469,14 +3432,8 @@
       <c r="Q14" t="s">
         <v>422</v>
       </c>
-      <c r="X14" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>236</v>
       </c>
@@ -3498,14 +3455,8 @@
       <c r="I15" t="s">
         <v>413</v>
       </c>
-      <c r="X15" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>108</v>
       </c>
@@ -3527,14 +3478,8 @@
       <c r="I16" t="s">
         <v>413</v>
       </c>
-      <c r="X16" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="17" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>110</v>
       </c>
@@ -3556,14 +3501,8 @@
       <c r="I17" t="s">
         <v>413</v>
       </c>
-      <c r="X17" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="18" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -3585,14 +3524,8 @@
       <c r="I18" t="s">
         <v>413</v>
       </c>
-      <c r="X18" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="19" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>114</v>
       </c>
@@ -3614,14 +3547,8 @@
       <c r="I19" t="s">
         <v>413</v>
       </c>
-      <c r="X19" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y19" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="20" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>116</v>
       </c>
@@ -3643,14 +3570,8 @@
       <c r="I20" t="s">
         <v>413</v>
       </c>
-      <c r="X20" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y20" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="21" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>118</v>
       </c>
@@ -3672,14 +3593,8 @@
       <c r="I21" t="s">
         <v>413</v>
       </c>
-      <c r="X21" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="22" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>142</v>
       </c>
@@ -3701,14 +3616,8 @@
       <c r="I22" t="s">
         <v>452</v>
       </c>
-      <c r="X22" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="23" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>44</v>
       </c>
@@ -3737,7 +3646,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="24" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>158</v>
       </c>
@@ -3766,7 +3675,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="25" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>160</v>
       </c>
@@ -3795,7 +3704,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="26" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>206</v>
       </c>
@@ -3817,14 +3726,8 @@
       <c r="I26" t="s">
         <v>454</v>
       </c>
-      <c r="X26" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="27" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -3846,14 +3749,8 @@
       <c r="I27" t="s">
         <v>413</v>
       </c>
-      <c r="X27" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="28" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>200</v>
       </c>
@@ -3875,14 +3772,8 @@
       <c r="I28" t="s">
         <v>455</v>
       </c>
-      <c r="X28" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="29" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -3907,14 +3798,8 @@
       <c r="I29" t="s">
         <v>413</v>
       </c>
-      <c r="X29" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="30" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>30</v>
       </c>
@@ -3939,14 +3824,8 @@
       <c r="I30" t="s">
         <v>413</v>
       </c>
-      <c r="X30" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="31" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>24</v>
       </c>
@@ -3971,14 +3850,8 @@
       <c r="I31" t="s">
         <v>413</v>
       </c>
-      <c r="X31" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y31" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="32" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -4003,14 +3876,8 @@
       <c r="I32" t="s">
         <v>413</v>
       </c>
-      <c r="X32" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y32" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>28</v>
       </c>
@@ -4035,14 +3902,8 @@
       <c r="I33" t="s">
         <v>413</v>
       </c>
-      <c r="X33" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y33" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -4067,14 +3928,8 @@
       <c r="I34" t="s">
         <v>413</v>
       </c>
-      <c r="X34" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="35" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>559</v>
       </c>
@@ -4105,14 +3960,8 @@
       <c r="O35" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="X35" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y35" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>559</v>
       </c>
@@ -4143,14 +3992,8 @@
       <c r="O36" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="X36" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y36" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>559</v>
       </c>
@@ -4181,14 +4024,8 @@
       <c r="O37" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="X37" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y37" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>104</v>
       </c>
@@ -4216,14 +4053,8 @@
       <c r="K38">
         <v>2010</v>
       </c>
-      <c r="X38" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>106</v>
       </c>
@@ -4248,14 +4079,8 @@
       <c r="J39">
         <v>6</v>
       </c>
-      <c r="X39" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y39" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -4277,14 +4102,8 @@
       <c r="I40" t="s">
         <v>427</v>
       </c>
-      <c r="X40" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>102</v>
       </c>
@@ -4306,14 +4125,8 @@
       <c r="I41" t="s">
         <v>413</v>
       </c>
-      <c r="X41" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y41" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>122</v>
       </c>
@@ -4344,14 +4157,8 @@
       <c r="O42" t="s">
         <v>463</v>
       </c>
-      <c r="X42" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>124</v>
       </c>
@@ -4382,14 +4189,8 @@
       <c r="O43" t="s">
         <v>465</v>
       </c>
-      <c r="X43" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>126</v>
       </c>
@@ -4420,14 +4221,8 @@
       <c r="O44" t="s">
         <v>466</v>
       </c>
-      <c r="X44" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>254</v>
       </c>
@@ -4458,14 +4253,8 @@
       <c r="O45" t="s">
         <v>467</v>
       </c>
-      <c r="X45" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>128</v>
       </c>
@@ -4496,14 +4285,8 @@
       <c r="O46" t="s">
         <v>468</v>
       </c>
-      <c r="X46" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>291</v>
       </c>
@@ -4534,14 +4317,8 @@
       <c r="O47" t="s">
         <v>469</v>
       </c>
-      <c r="X47" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>138</v>
       </c>
@@ -4572,14 +4349,8 @@
       <c r="O48" t="s">
         <v>470</v>
       </c>
-      <c r="X48" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="49" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>132</v>
       </c>
@@ -4610,14 +4381,8 @@
       <c r="O49" t="s">
         <v>471</v>
       </c>
-      <c r="X49" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="50" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>224</v>
       </c>
@@ -4648,14 +4413,8 @@
       <c r="O50" t="s">
         <v>472</v>
       </c>
-      <c r="X50" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="51" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>140</v>
       </c>
@@ -4686,14 +4445,8 @@
       <c r="O51" t="s">
         <v>473</v>
       </c>
-      <c r="X51" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="52" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>130</v>
       </c>
@@ -4724,14 +4477,8 @@
       <c r="O52" t="s">
         <v>474</v>
       </c>
-      <c r="X52" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="53" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>293</v>
       </c>
@@ -4762,14 +4509,8 @@
       <c r="O53" t="s">
         <v>475</v>
       </c>
-      <c r="X53" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="54" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>134</v>
       </c>
@@ -4800,14 +4541,8 @@
       <c r="O54" t="s">
         <v>476</v>
       </c>
-      <c r="X54" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="55" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>136</v>
       </c>
@@ -4838,14 +4573,8 @@
       <c r="O55" t="s">
         <v>477</v>
       </c>
-      <c r="X55" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="56" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>279</v>
       </c>
@@ -4876,14 +4605,8 @@
       <c r="O56" t="s">
         <v>478</v>
       </c>
-      <c r="X56" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="57" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>18</v>
       </c>
@@ -4908,14 +4631,8 @@
       <c r="K57" t="s">
         <v>423</v>
       </c>
-      <c r="X57" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="58" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>98</v>
       </c>
@@ -4940,14 +4657,8 @@
       <c r="K58" t="s">
         <v>423</v>
       </c>
-      <c r="X58" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y58" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="59" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>305</v>
       </c>
@@ -4982,7 +4693,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="60" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>303</v>
       </c>
@@ -5017,7 +4728,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="61" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>301</v>
       </c>
@@ -5052,7 +4763,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="62" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>311</v>
       </c>
@@ -5087,7 +4798,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="63" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>309</v>
       </c>
@@ -5122,7 +4833,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="64" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>307</v>
       </c>
@@ -5157,7 +4868,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="65" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>317</v>
       </c>
@@ -5192,7 +4903,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="66" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>315</v>
       </c>
@@ -5227,7 +4938,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="67" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>313</v>
       </c>
@@ -5255,14 +4966,8 @@
       <c r="O67" t="s">
         <v>446</v>
       </c>
-      <c r="X67" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y67" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="68" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>190</v>
       </c>
@@ -5287,14 +4992,8 @@
       <c r="J68">
         <v>6</v>
       </c>
-      <c r="X68" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y68" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="69" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>192</v>
       </c>
@@ -5319,14 +5018,8 @@
       <c r="J69">
         <v>6</v>
       </c>
-      <c r="X69" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y69" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="70" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>162</v>
       </c>
@@ -5351,14 +5044,8 @@
       <c r="J70">
         <v>3</v>
       </c>
-      <c r="X70" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y70" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="71" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>164</v>
       </c>
@@ -5383,14 +5070,8 @@
       <c r="J71">
         <v>3</v>
       </c>
-      <c r="X71" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="72" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>144</v>
       </c>
@@ -5415,14 +5096,8 @@
       <c r="J72">
         <v>3</v>
       </c>
-      <c r="X72" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y72" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="73" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>146</v>
       </c>
@@ -5447,14 +5122,8 @@
       <c r="J73">
         <v>3</v>
       </c>
-      <c r="X73" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y73" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="74" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>48</v>
       </c>
@@ -5479,14 +5148,8 @@
       <c r="J74">
         <v>6</v>
       </c>
-      <c r="X74" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y74" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="75" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>50</v>
       </c>
@@ -5511,14 +5174,8 @@
       <c r="J75">
         <v>6</v>
       </c>
-      <c r="X75" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y75" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="76" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>52</v>
       </c>
@@ -5543,14 +5200,8 @@
       <c r="J76">
         <v>3</v>
       </c>
-      <c r="X76" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y76" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="77" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>54</v>
       </c>
@@ -5575,14 +5226,8 @@
       <c r="J77">
         <v>6</v>
       </c>
-      <c r="X77" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y77" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="78" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>56</v>
       </c>
@@ -5607,14 +5252,8 @@
       <c r="J78">
         <v>6</v>
       </c>
-      <c r="X78" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y78" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="79" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>58</v>
       </c>
@@ -5639,14 +5278,8 @@
       <c r="J79">
         <v>6</v>
       </c>
-      <c r="X79" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y79" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="80" spans="2:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>60</v>
       </c>
@@ -5671,14 +5304,8 @@
       <c r="J80">
         <v>3</v>
       </c>
-      <c r="X80" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="81" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>62</v>
       </c>
@@ -5703,14 +5330,8 @@
       <c r="J81">
         <v>6</v>
       </c>
-      <c r="X81" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y81" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="82" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>285</v>
       </c>
@@ -5732,14 +5353,8 @@
       <c r="I82" t="s">
         <v>413</v>
       </c>
-      <c r="X82" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="83" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>148</v>
       </c>
@@ -5764,14 +5379,8 @@
       <c r="J83">
         <v>3</v>
       </c>
-      <c r="X83" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y83" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="84" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -5793,14 +5402,8 @@
       <c r="I84" t="s">
         <v>413</v>
       </c>
-      <c r="X84" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y84" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="85" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>222</v>
       </c>
@@ -5825,14 +5428,8 @@
       <c r="J85">
         <v>3</v>
       </c>
-      <c r="X85" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y85" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="86" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>46</v>
       </c>
@@ -5854,14 +5451,8 @@
       <c r="I86" t="s">
         <v>413</v>
       </c>
-      <c r="X86" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y86" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="87" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>559</v>
       </c>
@@ -5889,14 +5480,8 @@
       <c r="J87" s="1">
         <v>3</v>
       </c>
-      <c r="X87" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y87" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="88" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>287</v>
       </c>
@@ -5918,14 +5503,8 @@
       <c r="I88" t="s">
         <v>413</v>
       </c>
-      <c r="X88" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y88" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="89" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>150</v>
       </c>
@@ -5950,14 +5529,8 @@
       <c r="J89">
         <v>3</v>
       </c>
-      <c r="X89" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y89" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="90" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>323</v>
       </c>
@@ -5979,14 +5552,8 @@
       <c r="I90" t="s">
         <v>494</v>
       </c>
-      <c r="X90" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y90" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="91" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>321</v>
       </c>
@@ -6008,14 +5575,8 @@
       <c r="I91" t="s">
         <v>494</v>
       </c>
-      <c r="X91" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y91" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="92" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>319</v>
       </c>
@@ -6037,14 +5598,8 @@
       <c r="I92" t="s">
         <v>494</v>
       </c>
-      <c r="X92" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="93" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>327</v>
       </c>
@@ -6066,14 +5621,8 @@
       <c r="I93" t="s">
         <v>495</v>
       </c>
-      <c r="X93" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y93" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="94" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>325</v>
       </c>
@@ -6095,14 +5644,8 @@
       <c r="I94" t="s">
         <v>494</v>
       </c>
-      <c r="X94" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y94" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="95" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>178</v>
       </c>
@@ -6137,7 +5680,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="96" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>176</v>
       </c>
@@ -6172,7 +5715,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="97" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>182</v>
       </c>
@@ -6207,7 +5750,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="98" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>180</v>
       </c>
@@ -6242,7 +5785,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="99" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>186</v>
       </c>
@@ -6277,7 +5820,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="100" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>184</v>
       </c>
@@ -6312,7 +5855,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="101" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>188</v>
       </c>
@@ -6347,7 +5890,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="102" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>166</v>
       </c>
@@ -6369,14 +5912,8 @@
       <c r="I102" t="s">
         <v>420</v>
       </c>
-      <c r="X102" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y102" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="103" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>168</v>
       </c>
@@ -6398,14 +5935,8 @@
       <c r="I103" t="s">
         <v>420</v>
       </c>
-      <c r="X103" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y103" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="104" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>238</v>
       </c>
@@ -6427,14 +5958,8 @@
       <c r="I104" t="s">
         <v>515</v>
       </c>
-      <c r="X104" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y104" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="105" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>559</v>
       </c>
@@ -6465,14 +5990,8 @@
       <c r="J105" s="1">
         <v>6</v>
       </c>
-      <c r="X105" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y105" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="106" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>559</v>
       </c>
@@ -6503,14 +6022,8 @@
       <c r="J106" s="1">
         <v>6</v>
       </c>
-      <c r="X106" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y106" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="107" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>559</v>
       </c>
@@ -6541,14 +6054,8 @@
       <c r="J107" s="1">
         <v>6</v>
       </c>
-      <c r="X107" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y107" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="108" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>559</v>
       </c>
@@ -6576,14 +6083,8 @@
       <c r="J108" s="1">
         <v>6</v>
       </c>
-      <c r="X108" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y108" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="109" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>559</v>
       </c>
@@ -6611,14 +6112,8 @@
       <c r="J109" s="1">
         <v>6</v>
       </c>
-      <c r="X109" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y109" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="110" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>559</v>
       </c>
@@ -6646,14 +6141,8 @@
       <c r="J110" s="1">
         <v>6</v>
       </c>
-      <c r="X110" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y110" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="111" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>559</v>
       </c>
@@ -6681,14 +6170,8 @@
       <c r="I111" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="X111" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y111" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="112" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>559</v>
       </c>
@@ -6716,14 +6199,8 @@
       <c r="I112" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="X112" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y112" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="113" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>72</v>
       </c>
@@ -6754,14 +6231,8 @@
       <c r="S113" t="s">
         <v>434</v>
       </c>
-      <c r="X113" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y113" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="114" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>74</v>
       </c>
@@ -6792,14 +6263,8 @@
       <c r="S114" t="s">
         <v>435</v>
       </c>
-      <c r="X114" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y114" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>277</v>
       </c>
@@ -6827,14 +6292,8 @@
       <c r="S115" t="s">
         <v>418</v>
       </c>
-      <c r="X115" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y115" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="116" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>76</v>
       </c>
@@ -6865,14 +6324,8 @@
       <c r="S116" t="s">
         <v>418</v>
       </c>
-      <c r="X116" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y116" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="117" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>359</v>
       </c>
@@ -6894,14 +6347,8 @@
       <c r="I117" t="s">
         <v>420</v>
       </c>
-      <c r="X117" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y117" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="118" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>559</v>
       </c>
@@ -6933,7 +6380,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="119" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>559</v>
       </c>
@@ -6965,7 +6412,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="120" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>559</v>
       </c>
@@ -6997,7 +6444,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="121" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>559</v>
       </c>
@@ -7029,7 +6476,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="122" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>559</v>
       </c>
@@ -7054,14 +6501,8 @@
       <c r="I122" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="X122" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y122" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="123" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>559</v>
       </c>
@@ -7086,14 +6527,8 @@
       <c r="I123" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="X123" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y123" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="124" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>559</v>
       </c>
@@ -7118,14 +6553,8 @@
       <c r="I124" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="X124" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y124" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="125" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>559</v>
       </c>
@@ -7153,14 +6582,8 @@
       <c r="I125" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="X125" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y125" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="126" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>559</v>
       </c>
@@ -7188,14 +6611,8 @@
       <c r="I126" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="X126" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y126" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="127" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>559</v>
       </c>
@@ -7226,14 +6643,8 @@
       <c r="J127" s="1">
         <v>3</v>
       </c>
-      <c r="X127" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y127" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="128" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>559</v>
       </c>
@@ -7264,14 +6675,8 @@
       <c r="U128" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="X128" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y128" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="129" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>559</v>
       </c>
@@ -7302,14 +6707,8 @@
       <c r="U129" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="X129" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y129" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="130" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>559</v>
       </c>
@@ -7340,14 +6739,8 @@
       <c r="U130" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="X130" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y130" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="131" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>8</v>
       </c>
@@ -7375,14 +6768,8 @@
       <c r="U131" t="s">
         <v>417</v>
       </c>
-      <c r="X131" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y131" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="132" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>10</v>
       </c>
@@ -7410,14 +6797,8 @@
       <c r="U132" t="s">
         <v>418</v>
       </c>
-      <c r="X132" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y132" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="133" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>6</v>
       </c>
@@ -7445,14 +6826,8 @@
       <c r="U133" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="X133" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y133" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="134" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>14</v>
       </c>
@@ -7480,14 +6855,8 @@
       <c r="U134" t="s">
         <v>417</v>
       </c>
-      <c r="X134" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y134" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="135" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>16</v>
       </c>
@@ -7515,14 +6884,8 @@
       <c r="U135" t="s">
         <v>418</v>
       </c>
-      <c r="X135" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y135" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>12</v>
       </c>
@@ -7550,14 +6913,8 @@
       <c r="U136" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="X136" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y136" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>64</v>
       </c>
@@ -7585,14 +6942,8 @@
       <c r="U137" t="s">
         <v>417</v>
       </c>
-      <c r="X137" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y137" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="138" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>68</v>
       </c>
@@ -7620,14 +6971,8 @@
       <c r="U138" t="s">
         <v>418</v>
       </c>
-      <c r="X138" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y138" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="139" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>66</v>
       </c>
@@ -7655,14 +7000,8 @@
       <c r="U139" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="X139" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y139" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="140" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>78</v>
       </c>
@@ -7690,14 +7029,8 @@
       <c r="U140" t="s">
         <v>417</v>
       </c>
-      <c r="X140" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y140" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="141" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>70</v>
       </c>
@@ -7725,14 +7058,8 @@
       <c r="U141" t="s">
         <v>418</v>
       </c>
-      <c r="X141" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y141" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="142" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>86</v>
       </c>
@@ -7760,14 +7087,8 @@
       <c r="U142" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="X142" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y142" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="143" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>559</v>
       </c>
@@ -7798,14 +7119,8 @@
       <c r="W143" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="X143" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y143" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="144" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>559</v>
       </c>
@@ -7836,14 +7151,8 @@
       <c r="W144" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="X144" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y144" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="145" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>559</v>
       </c>
@@ -7865,14 +7174,8 @@
       <c r="H145" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="X145" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y145" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="146" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>559</v>
       </c>
@@ -7907,7 +7210,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="147" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>559</v>
       </c>
@@ -7942,7 +7245,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="148" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>559</v>
       </c>
@@ -7977,7 +7280,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="149" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>559</v>
       </c>
@@ -8002,14 +7305,8 @@
       <c r="I149" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="X149" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y149" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="150" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>559</v>
       </c>
@@ -8037,14 +7334,8 @@
       <c r="J150" s="1">
         <v>3</v>
       </c>
-      <c r="X150" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="Y150" s="1" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="151" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>339</v>
       </c>
@@ -8073,7 +7364,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="152" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>337</v>
       </c>
@@ -8102,7 +7393,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>335</v>
       </c>
@@ -8131,7 +7422,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="154" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>333</v>
       </c>
@@ -8160,7 +7451,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="155" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>331</v>
       </c>
@@ -8189,7 +7480,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="156" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>329</v>
       </c>
@@ -8218,7 +7509,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="157" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>559</v>
       </c>
@@ -8244,7 +7535,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="158" spans="1:25" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>559</v>
       </c>
@@ -8270,7 +7561,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="159" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
         <v>345</v>
       </c>
@@ -8293,7 +7584,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="160" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>347</v>
       </c>
@@ -8319,7 +7610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>371</v>
       </c>
@@ -8342,7 +7633,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="162" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>365</v>
       </c>
@@ -8365,7 +7656,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="163" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>373</v>
       </c>
@@ -8388,7 +7679,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="164" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>367</v>
       </c>
@@ -8417,7 +7708,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="165" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
         <v>369</v>
       </c>
@@ -8446,7 +7737,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="166" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
         <v>379</v>
       </c>
@@ -8469,7 +7760,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="167" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>377</v>
       </c>
@@ -8492,7 +7783,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="168" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
         <v>375</v>
       </c>
@@ -8515,7 +7806,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="169" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
         <v>256</v>
       </c>
@@ -8538,7 +7829,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="170" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
         <v>220</v>
       </c>
@@ -8561,7 +7852,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="171" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
         <v>218</v>
       </c>
@@ -8584,7 +7875,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="172" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
         <v>399</v>
       </c>
@@ -8607,7 +7898,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="173" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>403</v>
       </c>
@@ -8630,7 +7921,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="174" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>401</v>
       </c>
@@ -8653,7 +7944,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="175" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>391</v>
       </c>
@@ -8682,7 +7973,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="176" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>393</v>
       </c>
@@ -8711,7 +8002,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="177" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
         <v>395</v>
       </c>
@@ -8740,7 +8031,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="178" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
         <v>397</v>
       </c>
@@ -8769,7 +8060,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="179" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
         <v>387</v>
       </c>
@@ -8798,7 +8089,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="180" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>389</v>
       </c>
@@ -8827,7 +8118,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="181" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>226</v>
       </c>
@@ -8856,7 +8147,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="182" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>228</v>
       </c>
@@ -8885,7 +8176,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="183" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>230</v>
       </c>
@@ -8914,7 +8205,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="184" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
         <v>232</v>
       </c>
@@ -8940,7 +8231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>234</v>
       </c>
@@ -8969,7 +8260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>281</v>
       </c>
@@ -8992,7 +8283,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="187" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>283</v>
       </c>
@@ -9015,7 +8306,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="188" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>240</v>
       </c>
@@ -9041,7 +8332,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="189" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>242</v>
       </c>
@@ -9070,7 +8361,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="190" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
         <v>244</v>
       </c>
@@ -9099,7 +8390,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="191" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>246</v>
       </c>
@@ -9128,7 +8419,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="192" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>248</v>
       </c>
@@ -9157,7 +8448,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="193" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>250</v>
       </c>
@@ -9186,7 +8477,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="194" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>252</v>
       </c>
@@ -9215,7 +8506,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="195" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
         <v>257</v>
       </c>
@@ -9244,7 +8535,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
         <v>259</v>
       </c>
@@ -9273,7 +8564,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="197" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
         <v>261</v>
       </c>
@@ -9302,7 +8593,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="198" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
         <v>267</v>
       </c>
@@ -9331,7 +8622,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="199" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
         <v>265</v>
       </c>
@@ -9360,7 +8651,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="200" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B200" t="s">
         <v>263</v>
       </c>
@@ -9389,7 +8680,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="201" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B201" t="s">
         <v>269</v>
       </c>
@@ -9418,7 +8709,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="202" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
         <v>271</v>
       </c>
@@ -9447,7 +8738,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="203" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
         <v>275</v>
       </c>
@@ -9473,7 +8764,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="2:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B204" t="s">
         <v>273</v>
       </c>
@@ -9497,13 +8788,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB204" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="68"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB204" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="B2:AA204">
     <sortCondition ref="G2:G204"/>
     <sortCondition ref="E2:E204"/>

</xml_diff>

<commit_message>
syb country profile builder (selection of syb series)
</commit_message>
<xml_diff>
--- a/data/unsd/UNSYB/input/SYB series mapping to DSD.xlsx
+++ b/data/unsd/UNSYB/input/SYB series mapping to DSD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\data\unsd\UNSYB\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8E8795-C995-47A6-B208-FE75B8712ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BA5CAB-FA96-46B7-B9A0-8A211FE2A5A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SYB series mapping to DSD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="676">
   <si>
     <t>seriesCode</t>
   </si>
@@ -2909,26 +2909,26 @@
   <dimension ref="A1:AA204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="V35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
+      <selection pane="bottomRight" activeCell="X67" sqref="X67:Y67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="112.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="74.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="112.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="18" width="15.6640625" customWidth="1"/>
-    <col min="19" max="27" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="27" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>558</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>405</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>381</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>407</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>383</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>409</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>385</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>82</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>84</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>194</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>196</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>198</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>236</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>108</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>110</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>112</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>114</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>116</v>
       </c>
@@ -3571,7 +3571,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>118</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>142</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>44</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>158</v>
       </c>
@@ -3675,7 +3675,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>160</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>206</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>200</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>22</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>30</v>
       </c>
@@ -3825,7 +3825,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>24</v>
       </c>
@@ -3851,7 +3851,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>34</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>28</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>36</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>559</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>559</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>559</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>104</v>
       </c>
@@ -4054,7 +4054,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>106</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>100</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>102</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>122</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>124</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>126</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>254</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>128</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>291</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>138</v>
       </c>
@@ -4350,7 +4350,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>132</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>224</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>140</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>130</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>293</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>134</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>136</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>279</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>18</v>
       </c>
@@ -4632,7 +4632,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>98</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>305</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>303</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>301</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>311</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>309</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>307</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>317</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>315</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>313</v>
       </c>
@@ -4966,8 +4966,14 @@
       <c r="O67" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="X67" t="s">
+        <v>579</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>190</v>
       </c>
@@ -4993,7 +4999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>192</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>162</v>
       </c>
@@ -5045,7 +5051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>164</v>
       </c>
@@ -5071,7 +5077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>144</v>
       </c>
@@ -5097,7 +5103,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>146</v>
       </c>
@@ -5123,7 +5129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>48</v>
       </c>
@@ -5149,7 +5155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>50</v>
       </c>
@@ -5175,7 +5181,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>52</v>
       </c>
@@ -5201,7 +5207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>54</v>
       </c>
@@ -5227,7 +5233,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>56</v>
       </c>
@@ -5253,7 +5259,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>58</v>
       </c>
@@ -5279,7 +5285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>60</v>
       </c>
@@ -5305,7 +5311,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>62</v>
       </c>
@@ -5331,7 +5337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>285</v>
       </c>
@@ -5354,7 +5360,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>148</v>
       </c>
@@ -5380,7 +5386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -5403,7 +5409,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>222</v>
       </c>
@@ -5429,7 +5435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>46</v>
       </c>
@@ -5452,7 +5458,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="87" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>559</v>
       </c>
@@ -5481,7 +5487,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>287</v>
       </c>
@@ -5504,7 +5510,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>150</v>
       </c>
@@ -5530,7 +5536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>323</v>
       </c>
@@ -5553,7 +5559,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>321</v>
       </c>
@@ -5576,7 +5582,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>319</v>
       </c>
@@ -5599,7 +5605,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>327</v>
       </c>
@@ -5622,7 +5628,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>325</v>
       </c>
@@ -5645,7 +5651,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>178</v>
       </c>
@@ -5680,7 +5686,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>176</v>
       </c>
@@ -5715,7 +5721,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>182</v>
       </c>
@@ -5750,7 +5756,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>180</v>
       </c>
@@ -5785,7 +5791,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>186</v>
       </c>
@@ -5820,7 +5826,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>184</v>
       </c>
@@ -5855,7 +5861,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>188</v>
       </c>
@@ -5890,7 +5896,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>166</v>
       </c>
@@ -5913,7 +5919,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>168</v>
       </c>
@@ -5936,7 +5942,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>238</v>
       </c>
@@ -5959,7 +5965,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="105" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>559</v>
       </c>
@@ -5991,7 +5997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>559</v>
       </c>
@@ -6023,7 +6029,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>559</v>
       </c>
@@ -6055,7 +6061,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>559</v>
       </c>
@@ -6084,7 +6090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>559</v>
       </c>
@@ -6113,7 +6119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>559</v>
       </c>
@@ -6142,7 +6148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>559</v>
       </c>
@@ -6171,7 +6177,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="112" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>559</v>
       </c>
@@ -6200,7 +6206,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>72</v>
       </c>
@@ -6232,7 +6238,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>74</v>
       </c>
@@ -6264,7 +6270,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>277</v>
       </c>
@@ -6293,7 +6299,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>76</v>
       </c>
@@ -6325,7 +6331,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>359</v>
       </c>
@@ -6348,7 +6354,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>559</v>
       </c>
@@ -6380,7 +6386,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="119" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>559</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="120" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>559</v>
       </c>
@@ -6444,7 +6450,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="121" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>559</v>
       </c>
@@ -6476,7 +6482,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="122" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>559</v>
       </c>
@@ -6502,7 +6508,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="123" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>559</v>
       </c>
@@ -6528,7 +6534,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="124" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>559</v>
       </c>
@@ -6554,7 +6560,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="125" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>559</v>
       </c>
@@ -6583,7 +6589,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="126" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>559</v>
       </c>
@@ -6612,7 +6618,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="127" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>559</v>
       </c>
@@ -6644,7 +6650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>559</v>
       </c>
@@ -6676,7 +6682,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="129" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>559</v>
       </c>
@@ -6708,7 +6714,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="130" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>559</v>
       </c>
@@ -6740,7 +6746,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>8</v>
       </c>
@@ -6769,7 +6775,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>10</v>
       </c>
@@ -6798,7 +6804,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>6</v>
       </c>
@@ -6827,7 +6833,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>14</v>
       </c>
@@ -6856,7 +6862,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>16</v>
       </c>
@@ -6885,7 +6891,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>12</v>
       </c>
@@ -6914,7 +6920,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>64</v>
       </c>
@@ -6943,7 +6949,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>68</v>
       </c>
@@ -6972,7 +6978,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>66</v>
       </c>
@@ -7001,7 +7007,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>78</v>
       </c>
@@ -7030,7 +7036,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>70</v>
       </c>
@@ -7059,7 +7065,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>86</v>
       </c>
@@ -7088,7 +7094,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="143" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>559</v>
       </c>
@@ -7120,7 +7126,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="144" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>559</v>
       </c>
@@ -7152,7 +7158,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="145" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>559</v>
       </c>
@@ -7175,7 +7181,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="146" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>559</v>
       </c>
@@ -7210,7 +7216,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="147" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>559</v>
       </c>
@@ -7245,7 +7251,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="148" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>559</v>
       </c>
@@ -7280,7 +7286,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="149" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>559</v>
       </c>
@@ -7306,7 +7312,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="150" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>559</v>
       </c>
@@ -7335,7 +7341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>339</v>
       </c>
@@ -7364,7 +7370,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>337</v>
       </c>
@@ -7393,7 +7399,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>335</v>
       </c>
@@ -7422,7 +7428,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>333</v>
       </c>
@@ -7451,7 +7457,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>331</v>
       </c>
@@ -7480,7 +7486,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>329</v>
       </c>
@@ -7509,7 +7515,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="157" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>559</v>
       </c>
@@ -7535,7 +7541,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="158" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>559</v>
       </c>
@@ -7561,7 +7567,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>345</v>
       </c>
@@ -7584,7 +7590,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
         <v>347</v>
       </c>
@@ -7610,7 +7616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
         <v>371</v>
       </c>
@@ -7633,7 +7639,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="162" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
         <v>365</v>
       </c>
@@ -7656,7 +7662,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="163" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
         <v>373</v>
       </c>
@@ -7679,7 +7685,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="164" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
         <v>367</v>
       </c>
@@ -7708,7 +7714,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="165" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>369</v>
       </c>
@@ -7737,7 +7743,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="166" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
         <v>379</v>
       </c>
@@ -7760,7 +7766,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="167" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
         <v>377</v>
       </c>
@@ -7783,7 +7789,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="168" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
         <v>375</v>
       </c>
@@ -7806,7 +7812,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="169" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
         <v>256</v>
       </c>
@@ -7829,7 +7835,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="170" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>220</v>
       </c>
@@ -7852,7 +7858,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="171" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
         <v>218</v>
       </c>
@@ -7875,7 +7881,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="172" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>399</v>
       </c>
@@ -7898,7 +7904,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="173" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>403</v>
       </c>
@@ -7921,7 +7927,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="174" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
         <v>401</v>
       </c>
@@ -7944,7 +7950,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="175" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>391</v>
       </c>
@@ -7973,7 +7979,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="176" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>393</v>
       </c>
@@ -8002,7 +8008,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="177" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>395</v>
       </c>
@@ -8031,7 +8037,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="178" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
         <v>397</v>
       </c>
@@ -8060,7 +8066,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="179" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>387</v>
       </c>
@@ -8089,7 +8095,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="180" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
         <v>389</v>
       </c>
@@ -8118,7 +8124,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="181" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>226</v>
       </c>
@@ -8147,7 +8153,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="182" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
         <v>228</v>
       </c>
@@ -8176,7 +8182,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="183" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
         <v>230</v>
       </c>
@@ -8205,7 +8211,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="184" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>232</v>
       </c>
@@ -8231,7 +8237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>234</v>
       </c>
@@ -8260,7 +8266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
         <v>281</v>
       </c>
@@ -8283,7 +8289,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="187" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>283</v>
       </c>
@@ -8306,7 +8312,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="188" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
         <v>240</v>
       </c>
@@ -8332,7 +8338,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="189" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>242</v>
       </c>
@@ -8361,7 +8367,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="190" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
         <v>244</v>
       </c>
@@ -8390,7 +8396,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="191" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>246</v>
       </c>
@@ -8419,7 +8425,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="192" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
         <v>248</v>
       </c>
@@ -8448,7 +8454,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="193" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
         <v>250</v>
       </c>
@@ -8477,7 +8483,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="194" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>252</v>
       </c>
@@ -8506,7 +8512,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="195" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
         <v>257</v>
       </c>
@@ -8535,7 +8541,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
         <v>259</v>
       </c>
@@ -8564,7 +8570,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="197" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>261</v>
       </c>
@@ -8593,7 +8599,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="198" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
         <v>267</v>
       </c>
@@ -8622,7 +8628,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="199" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>265</v>
       </c>
@@ -8651,7 +8657,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="200" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>263</v>
       </c>
@@ -8680,7 +8686,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="201" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>269</v>
       </c>
@@ -8709,7 +8715,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="202" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
         <v>271</v>
       </c>
@@ -8738,7 +8744,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="203" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>275</v>
       </c>
@@ -8764,7 +8770,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="204" spans="2:27" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
         <v>273</v>
       </c>

</xml_diff>